<commit_message>
feat: Change the test to use currency conversion (MPT-8993)
</commit_message>
<xml_diff>
--- a/tests/commands/snapshots/test_generate_monthtly_charges/test_export_to_zip/charges_file.xlsx
+++ b/tests/commands/snapshots/test_generate_monthtly_charges/test_export_to_zip/charges_file.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="29">
   <si>
     <t>Entry ID</t>
   </si>
@@ -76,16 +76,16 @@
     <t>31-Mar-2025</t>
   </si>
   <si>
-    <t>0.60</t>
-  </si>
-  <si>
-    <t>-0.60</t>
-  </si>
-  <si>
-    <t>0.70</t>
-  </si>
-  <si>
-    <t>0.40</t>
+    <t>0.56</t>
+  </si>
+  <si>
+    <t>-0.56</t>
+  </si>
+  <si>
+    <t>0.65</t>
+  </si>
+  <si>
+    <t>-0.65</t>
   </si>
   <si>
     <t>9a1de644-815e-46d1-bb8f-aa1837f8a88b</t>
@@ -97,16 +97,10 @@
     <t>GCP Account</t>
   </si>
   <si>
-    <t>Azure Account</t>
-  </si>
-  <si>
     <t>b74d0fb1-32e7-4629-8fad-c1a606cb0fb3</t>
   </si>
   <si>
     <t>6b65a6a4-8b81-48f6-b38a-088ca65ed389</t>
-  </si>
-  <si>
-    <t>47378190-96da-4dac-b2ff-5d2a386ecbe0</t>
   </si>
 </sst>
 </file>
@@ -552,7 +546,7 @@
         <v>25</v>
       </c>
       <c r="M2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -593,7 +587,7 @@
         <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -634,7 +628,7 @@
         <v>26</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -672,10 +666,10 @@
         <v>24</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Upload charge files to Azure and save them in the db (MPT-8992, MPT-8994)
</commit_message>
<xml_diff>
--- a/tests/commands/snapshots/test_generate_monthtly_charges/test_export_to_zip/charges_file.xlsx
+++ b/tests/commands/snapshots/test_generate_monthtly_charges/test_export_to_zip/charges_file.xlsx
@@ -61,7 +61,7 @@
     <t>subscription.externalIds.vendor</t>
   </si>
   <si>
-    <t>FORG-2846-5181-3940</t>
+    <t>FORG-7330-1645-9608</t>
   </si>
   <si>
     <t>item.externalIds.vendor</t>
@@ -88,7 +88,7 @@
     <t>-0.65</t>
   </si>
   <si>
-    <t>9a1de644-815e-46d1-bb8f-aa1837f8a88b</t>
+    <t>06cb0fb3-9a1d-4644-815e-f6d13b8faa18</t>
   </si>
   <si>
     <t>AWS Account</t>
@@ -97,10 +97,10 @@
     <t>GCP Account</t>
   </si>
   <si>
-    <t>b74d0fb1-32e7-4629-8fad-c1a606cb0fb3</t>
-  </si>
-  <si>
-    <t>6b65a6a4-8b81-48f6-b38a-088ca65ed389</t>
+    <t>a65ed389-b74d-4fb1-b2e7-06298fadc1a6</t>
+  </si>
+  <si>
+    <t>386ecbe0-6b65-46a4-8b81-48f6b38a088c</t>
   </si>
 </sst>
 </file>

</xml_diff>